<commit_message>
Added Text Area Validation to DeleteEntry action. Added navigate to correct day to BeginEntry action.
Used Days in data table as the date link to click - not a good permanent solution, but works for now.
</commit_message>
<xml_diff>
--- a/Chronos/testdata.xlsx
+++ b/Chronos/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awalton\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awalton\Documents\GitHub\chronosUFT\Chronos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Computer Solutions Company</t>
   </si>
   <si>
-    <t>Skills Enhancement</t>
-  </si>
-  <si>
     <t>Human Resources</t>
   </si>
   <si>
@@ -75,6 +72,18 @@
   </si>
   <si>
     <t>Fun Team Event at Freedom Park</t>
+  </si>
+  <si>
+    <t>Skill Enhancement</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>UFT Training</t>
+  </si>
+  <si>
+    <t>Mandatory Fun</t>
   </si>
 </sst>
 </file>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +424,10 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="35.140625" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -439,8 +449,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42968</v>
       </c>
@@ -451,19 +464,22 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
+      <c r="H2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42969</v>
       </c>
@@ -474,19 +490,22 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42969</v>
       </c>
@@ -497,19 +516,22 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
+      <c r="H4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42970</v>
       </c>
@@ -520,19 +542,22 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42971</v>
       </c>
@@ -543,19 +568,22 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
-        <v>15</v>
+      <c r="H6" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42972</v>
       </c>
@@ -566,16 +594,19 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
-        <v>15</v>
+      <c r="H7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>